<commit_message>
Revised update of SLIM_Bitcoin_Compression_Result_Summary file
Revised update of SLIM_Bitcoin_Compression_Result_Summary file to correct % compression levels and include additional 10 minute bucket values of 16th December 2017 21:00 to 22:00
</commit_message>
<xml_diff>
--- a/SLIM_Bitcoin_Compression_Result_Summary.xlsx
+++ b/SLIM_Bitcoin_Compression_Result_Summary.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eoinc\Dropbox\PHD\My_Thesis\Viva_RW\Corrections_RW\Result_Excel_Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eoinc\Documents\GitHub\Slim-Thesis-Result-Set\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A97D960-A4A5-404F-A3AE-F1D370CCF79F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F61660C0-3B60-4843-A834-57AE0E66A7B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8295" yWindow="4545" windowWidth="23250" windowHeight="14970" tabRatio="815" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6450" yWindow="4110" windowWidth="23250" windowHeight="14970" tabRatio="815" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Day Level" sheetId="16" r:id="rId1"/>
@@ -696,7 +696,7 @@
   </sheetPr>
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
@@ -899,7 +899,7 @@
   </sheetPr>
   <dimension ref="A2:Q27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
@@ -2219,8 +2219,8 @@
   </sheetPr>
   <dimension ref="A2:Q24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2931,7 +2931,7 @@
         <v>0.52300000000000002</v>
       </c>
       <c r="F16" s="5">
-        <v>6.69</v>
+        <v>52.300000000000004</v>
       </c>
       <c r="G16" s="4">
         <v>43.889699999999998</v>
@@ -2957,7 +2957,7 @@
         <v>0.56669999999999998</v>
       </c>
       <c r="F17" s="5">
-        <v>11.55</v>
+        <v>56.67</v>
       </c>
       <c r="G17" s="4">
         <v>5.9950000000000001</v>
@@ -2983,7 +2983,7 @@
         <v>0.46989999999999998</v>
       </c>
       <c r="F18" s="5">
-        <v>9.2899999999999991</v>
+        <v>46.989999999999995</v>
       </c>
       <c r="G18" s="4">
         <v>13.314399999999999</v>
@@ -3009,7 +3009,7 @@
         <v>0.49969999999999998</v>
       </c>
       <c r="F19" s="5">
-        <v>10.280000000000001</v>
+        <v>49.97</v>
       </c>
       <c r="G19" s="4">
         <v>12.843400000000001</v>
@@ -3035,7 +3035,7 @@
         <v>0.58660000000000001</v>
       </c>
       <c r="F20" s="5">
-        <v>10.8</v>
+        <v>58.660000000000004</v>
       </c>
       <c r="G20" s="4">
         <v>13.039099999999999</v>
@@ -3061,7 +3061,7 @@
         <v>0.54239999999999999</v>
       </c>
       <c r="F21" s="5">
-        <v>7.4399999999999995</v>
+        <v>54.24</v>
       </c>
       <c r="G21" s="4">
         <v>15.930400000000001</v>

</xml_diff>

<commit_message>
Update of December 16th 21:00hr 10 minute Raw series stdDev values
Update of December 16th 21:00hr 10 minute Raw series stdDev values as the wrong column was pasted in previous versions of teh Excel file
</commit_message>
<xml_diff>
--- a/SLIM_Bitcoin_Compression_Result_Summary.xlsx
+++ b/SLIM_Bitcoin_Compression_Result_Summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eoinc\Documents\GitHub\Slim-Thesis-Result-Set\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F61660C0-3B60-4843-A834-57AE0E66A7B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E7E234A4-DF24-49A9-92F1-EA278BE154E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6450" yWindow="4110" windowWidth="23250" windowHeight="14970" tabRatio="815" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="28800" windowHeight="18345" tabRatio="815" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Day Level" sheetId="16" r:id="rId1"/>
@@ -696,8 +696,8 @@
   </sheetPr>
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2219,8 +2219,8 @@
   </sheetPr>
   <dimension ref="A2:Q24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2928,13 +2928,13 @@
         <v>5.1799999999999999E-2</v>
       </c>
       <c r="E16" s="4">
-        <v>0.52300000000000002</v>
+        <v>43.889699999999998</v>
       </c>
       <c r="F16" s="5">
         <v>52.300000000000004</v>
       </c>
       <c r="G16" s="4">
-        <v>43.889699999999998</v>
+        <v>6.6900000000000001E-2</v>
       </c>
       <c r="H16" s="4">
         <v>2.0217999999999999E-4</v>
@@ -2954,13 +2954,13 @@
         <v>2.5399999999999999E-2</v>
       </c>
       <c r="E17" s="4">
-        <v>0.56669999999999998</v>
+        <v>5.9950000000000001</v>
       </c>
       <c r="F17" s="5">
         <v>56.67</v>
       </c>
       <c r="G17" s="4">
-        <v>5.9950000000000001</v>
+        <v>0.11550000000000001</v>
       </c>
       <c r="H17" s="4">
         <v>7.8407999999999999E-5</v>
@@ -2980,13 +2980,13 @@
         <v>2.92E-2</v>
       </c>
       <c r="E18" s="4">
-        <v>0.46989999999999998</v>
+        <v>13.314399999999999</v>
       </c>
       <c r="F18" s="5">
         <v>46.989999999999995</v>
       </c>
       <c r="G18" s="4">
-        <v>13.314399999999999</v>
+        <v>9.2899999999999996E-2</v>
       </c>
       <c r="H18" s="4">
         <v>3.8727999999999999E-5</v>
@@ -3006,13 +3006,13 @@
         <v>5.04E-2</v>
       </c>
       <c r="E19" s="4">
-        <v>0.49969999999999998</v>
+        <v>12.843400000000001</v>
       </c>
       <c r="F19" s="5">
         <v>49.97</v>
       </c>
       <c r="G19" s="4">
-        <v>12.843400000000001</v>
+        <v>0.1028</v>
       </c>
       <c r="H19" s="4">
         <v>1.7681000000000001E-4</v>
@@ -3032,13 +3032,13 @@
         <v>2.5700000000000001E-2</v>
       </c>
       <c r="E20" s="4">
-        <v>0.58660000000000001</v>
+        <v>13.039099999999999</v>
       </c>
       <c r="F20" s="5">
         <v>58.660000000000004</v>
       </c>
       <c r="G20" s="4">
-        <v>13.039099999999999</v>
+        <v>0.108</v>
       </c>
       <c r="H20" s="4">
         <v>1.0477E-4</v>
@@ -3058,13 +3058,13 @@
         <v>3.6499999999999998E-2</v>
       </c>
       <c r="E21" s="4">
-        <v>0.54239999999999999</v>
+        <v>15.930400000000001</v>
       </c>
       <c r="F21" s="5">
         <v>54.24</v>
       </c>
       <c r="G21" s="4">
-        <v>15.930400000000001</v>
+        <v>7.4399999999999994E-2</v>
       </c>
       <c r="H21" s="4">
         <v>1.5924E-4</v>

</xml_diff>